<commit_message>
feat: Git commands doc
</commit_message>
<xml_diff>
--- a/Document/web app tech-stack.xlsx
+++ b/Document/web app tech-stack.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18885" windowHeight="8385" activeTab="4"/>
+    <workbookView windowWidth="24000" windowHeight="9765"/>
   </bookViews>
   <sheets>
     <sheet name="Rendering Engine" sheetId="1" r:id="rId1"/>
@@ -265,10 +265,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -297,15 +297,40 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -319,6 +344,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
@@ -327,13 +375,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -342,14 +383,42 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -364,44 +433,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -409,37 +440,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -456,25 +456,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -486,157 +636,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -647,15 +647,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -674,37 +665,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -714,6 +685,15 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -733,17 +713,37 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -755,10 +755,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -767,133 +767,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1263,16 +1263,15 @@
   <sheetPr/>
   <dimension ref="B2:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
     <col min="2" max="2" width="9.125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.25" style="1" customWidth="1"/>
+    <col min="3" max="4" width="14.875" style="1" customWidth="1"/>
     <col min="5" max="16383" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -1740,7 +1739,7 @@
   <sheetPr/>
   <dimension ref="B1:XFD21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1815,8 +1814,6 @@
     </row>
     <row r="11" s="1" customFormat="1" spans="2:16384">
       <c r="B11" s="2"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
       <c r="XFD11"/>
     </row>
     <row r="12" s="1" customFormat="1" spans="16384:16384">

</xml_diff>